<commit_message>
Still working on spreadsheet
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="191">
   <si>
     <t>Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Medical</t>
   </si>
   <si>
-    <t>Action 1 Cost</t>
-  </si>
-  <si>
     <t>Chief</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Can only take actions with ➜, and no other subactions</t>
   </si>
   <si>
-    <t>Maximum of 1 Energy regain per round</t>
-  </si>
-  <si>
     <t>Lose 3 Energy</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Look</t>
   </si>
   <si>
-    <t>Sight</t>
-  </si>
-  <si>
     <t>➕</t>
   </si>
   <si>
@@ -263,9 +254,6 @@
     <t>Extinguisher</t>
   </si>
   <si>
-    <t>Wire Cutters</t>
-  </si>
-  <si>
     <t>Medkit</t>
   </si>
   <si>
@@ -491,9 +479,6 @@
     <t>Fully Buried Victim</t>
   </si>
   <si>
-    <t>Cannot treat the victim until they are cleared.</t>
-  </si>
-  <si>
     <t>"I think I see someone in there"</t>
   </si>
   <si>
@@ -543,6 +528,75 @@
   </si>
   <si>
     <t>Suicide Bomber</t>
+  </si>
+  <si>
+    <t>Speed is 1, cannot take actions with 3 or more subactions</t>
+  </si>
+  <si>
+    <t>Unearth%n💪 💪🔍</t>
+  </si>
+  <si>
+    <t>Assault%n🔫🔫</t>
+  </si>
+  <si>
+    <t>Clear%n💪</t>
+  </si>
+  <si>
+    <t>A1Cost</t>
+  </si>
+  <si>
+    <t>Bomb Shield</t>
+  </si>
+  <si>
+    <t>Contain%n☣</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Cannot treat the victim until they are cleared. Unless Handled, add 1 Treat on Rounds 5,6, and 7.</t>
+  </si>
+  <si>
+    <t>Debris Collapse</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Cthru</t>
+  </si>
+  <si>
+    <t>Hazard</t>
+  </si>
+  <si>
+    <t>Small Fire</t>
+  </si>
+  <si>
+    <t>Flaming Gas Can</t>
+  </si>
+  <si>
+    <t>Unless handled, add Extinguish at rounds 2, 3, and 5</t>
+  </si>
+  <si>
+    <t>Faulty Wiring</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reveal all cards when this is revealed. Add Extinguish </t>
+  </si>
+  <si>
+    <t>Shooter</t>
+  </si>
+  <si>
+    <t>Cannot exit until situation is handled</t>
+  </si>
+  <si>
+    <t>"How many more are there??"</t>
   </si>
 </sst>
 </file>
@@ -905,11 +959,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O8" sqref="O8"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,24 +972,23 @@
     <col min="2" max="2" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="76.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,55 +999,52 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1005,57 +1055,54 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="3">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="3">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="3">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>113</v>
-      </c>
-      <c r="P2" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="3">
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>169</v>
+      </c>
+      <c r="M2" s="3">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="3">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" s="3">
         <v>4</v>
       </c>
-      <c r="S2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1064,60 +1111,57 @@
         <v>6</v>
       </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="3">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="3">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P3" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
         <v>85</v>
       </c>
-      <c r="R3" s="3">
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" s="3">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q3" s="3">
         <v>5</v>
       </c>
-      <c r="S3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4" s="3">
         <v>5</v>
@@ -1126,49 +1170,49 @@
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" s="3">
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>87</v>
-      </c>
-      <c r="P4" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>85</v>
-      </c>
-      <c r="R4" s="3">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1179,57 +1223,54 @@
         <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J5" s="3">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L5" s="3">
-        <v>3</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="3">
-        <v>2</v>
-      </c>
-      <c r="O5" t="s">
-        <v>101</v>
-      </c>
-      <c r="P5" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="3">
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="3">
         <v>5</v>
       </c>
-      <c r="S5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1238,232 +1279,220 @@
         <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="3">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="3">
         <v>4</v>
       </c>
-      <c r="M6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" s="3">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="L6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="3">
         <v>4</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="P6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
         <v>85</v>
       </c>
-      <c r="R6" s="3">
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>169</v>
+      </c>
+      <c r="O7" s="3">
         <v>4</v>
       </c>
-      <c r="S6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="P7" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J7" s="3">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>125</v>
+      </c>
+      <c r="O8" s="3">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q8" s="3">
         <v>4</v>
       </c>
-      <c r="M7" t="s">
-        <v>87</v>
-      </c>
-      <c r="N7" s="3">
-        <v>2</v>
-      </c>
-      <c r="O7" t="s">
-        <v>104</v>
-      </c>
-      <c r="P7" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>85</v>
-      </c>
-      <c r="R7" s="3">
-        <v>5</v>
-      </c>
-      <c r="S7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="3">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L8" s="3">
-        <v>3</v>
-      </c>
-      <c r="M8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N8" s="3">
-        <v>2</v>
-      </c>
-      <c r="O8" t="s">
-        <v>129</v>
-      </c>
-      <c r="P8" s="3">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>85</v>
-      </c>
-      <c r="R8" s="3">
-        <v>4</v>
-      </c>
-      <c r="S8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="3">
-        <v>2</v>
-      </c>
-      <c r="K9" t="s">
-        <v>86</v>
-      </c>
-      <c r="L9" s="3">
-        <v>2</v>
-      </c>
-      <c r="M9" t="s">
-        <v>100</v>
-      </c>
-      <c r="N9" s="3">
-        <v>2</v>
-      </c>
-      <c r="O9" t="s">
-        <v>123</v>
-      </c>
-      <c r="P9" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="3">
+      <c r="I9" s="3">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>119</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q9" s="3">
         <v>6</v>
       </c>
-      <c r="S9" t="s">
-        <v>67</v>
+      <c r="R9" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 I5:I9 Q2:Q9 M2:M9 K2:K9 I3 O2:O9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9 H5:H9 P2:P9 L2:L9 H3 N2:N9 J2:J7 J9">
       <formula1>Action</formula1>
     </dataValidation>
   </dataValidations>
@@ -1482,7 +1511,7 @@
   <sheetData>
     <row r="3" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1492,290 +1521,410 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="45" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="6" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="S2" s="3">
+        <f>H2+J2+L2+N2+P2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="R2" s="3">
-        <f>G2+I2+K2+M2+O2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>149</v>
+        <v>179</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S4" si="0">H3+J3+L3+N3+P3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="R3" s="3">
-        <f t="shared" ref="R3:R4" si="0">G3+I3+K3+M3+O3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="R4" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="P12" s="5" t="s">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>172</v>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1789,7 +1938,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,10 +1949,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1811,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1819,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1827,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1835,7 +1984,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1843,7 +1992,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,7 +2000,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1859,7 +2008,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1872,14 +2021,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1889,97 +2038,100 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9 C6 C2:C5">
       <formula1>Action</formula1>
     </dataValidation>
   </dataValidations>
@@ -1990,70 +2142,136 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
+        <v>173</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C5">
+      <formula1>Action</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2064,7 +2282,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,137 +2292,137 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2220,7 +2438,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,145 +2450,145 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on jobs cards
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Jobs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="228">
   <si>
     <t>Name</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Action 2</t>
   </si>
   <si>
-    <t>Action2</t>
-  </si>
-  <si>
     <t>Action 3</t>
   </si>
   <si>
@@ -700,6 +697,18 @@
   </si>
   <si>
     <t>URGENT: Unless handled, add 1 Extinguish each round. If a colleague starts a round with 5 or more Extinguish needs on this card, add 1 Panic.</t>
+  </si>
+  <si>
+    <t>Leader</t>
+  </si>
+  <si>
+    <t>Medic</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>Civilian</t>
   </si>
 </sst>
 </file>
@@ -1063,540 +1072,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="76.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" s="3">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="3">
-        <v>3</v>
-      </c>
-      <c r="N2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O2" s="3">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="3">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="3">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="3">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="3">
-        <v>3</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R3" s="3">
         <v>5</v>
       </c>
-      <c r="R3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
       <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="3">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" s="3">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="3">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
-        <v>81</v>
-      </c>
-      <c r="O4" s="3">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>78</v>
+      </c>
+      <c r="R4" s="3">
+        <v>3</v>
+      </c>
+      <c r="S4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
       <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" s="3">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K5" s="3">
-        <v>3</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="3">
-        <v>2</v>
-      </c>
-      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
         <v>95</v>
       </c>
-      <c r="O5" s="3">
-        <v>3</v>
-      </c>
-      <c r="P5" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q5" s="3">
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="3">
         <v>5</v>
       </c>
-      <c r="R5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
-        <v>3</v>
+      <c r="C6" t="s">
+        <v>225</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+      <c r="O6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="3">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
         <v>119</v>
       </c>
-      <c r="G6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="3">
-        <v>2</v>
-      </c>
-      <c r="J6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K6" s="3">
-        <v>4</v>
-      </c>
-      <c r="L6" t="s">
-        <v>107</v>
-      </c>
-      <c r="M6" s="3">
-        <v>2</v>
-      </c>
-      <c r="N6" t="s">
-        <v>94</v>
-      </c>
-      <c r="O6" s="3">
-        <v>4</v>
-      </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>4</v>
-      </c>
-      <c r="R6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
-        <v>2</v>
+      <c r="C7" t="s">
+        <v>226</v>
       </c>
       <c r="D7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="3">
-        <v>3</v>
-      </c>
-      <c r="L7" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="3">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>163</v>
-      </c>
-      <c r="O7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="3">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>162</v>
+      </c>
+      <c r="P7" s="3">
         <v>4</v>
       </c>
-      <c r="P7" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="Q7" t="s">
+        <v>78</v>
+      </c>
+      <c r="R7" s="3">
         <v>5</v>
       </c>
-      <c r="R7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
-        <v>3</v>
+      <c r="C8" t="s">
+        <v>226</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="3">
-        <v>2</v>
-      </c>
-      <c r="J8" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="3">
-        <v>3</v>
-      </c>
-      <c r="L8" t="s">
-        <v>81</v>
-      </c>
-      <c r="M8" s="3">
-        <v>2</v>
-      </c>
-      <c r="N8" t="s">
-        <v>122</v>
-      </c>
-      <c r="O8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="3">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>121</v>
+      </c>
+      <c r="P8" s="3">
         <v>5</v>
       </c>
-      <c r="P8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="3">
         <v>4</v>
       </c>
-      <c r="R8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" s="3">
-        <v>2</v>
-      </c>
-      <c r="J9" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="3">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="3">
-        <v>2</v>
-      </c>
-      <c r="N9" t="s">
-        <v>116</v>
-      </c>
-      <c r="O9" s="3">
-        <v>1</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
         <v>79</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="L9" s="3">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" t="s">
+        <v>115</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="3">
         <v>6</v>
       </c>
-      <c r="R9" t="s">
-        <v>63</v>
+      <c r="S9" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9 H5:H9 P2:P9 L2:L9 H3 N2:N9 J2:J7 J9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 I5:I9 Q2:Q9 M2:M9 I3 O2:O9 K2:K7 K9">
       <formula1>Action</formula1>
     </dataValidation>
   </dataValidations>
@@ -1625,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -1636,88 +1673,88 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" t="s">
         <v>186</v>
-      </c>
-      <c r="D4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
         <v>188</v>
-      </c>
-      <c r="D5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
         <v>191</v>
-      </c>
-      <c r="B7" t="s">
-        <v>192</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" t="s">
         <v>194</v>
-      </c>
-      <c r="D8" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>197</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
         <v>199</v>
-      </c>
-      <c r="D11" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1735,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,87 +1805,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3">
         <v>2</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S2" s="3">
         <f>H2+J2+L2+N2+P2</f>
@@ -1857,31 +1894,31 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="R3" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S3" s="3">
         <f t="shared" ref="S3:S25" si="0">H3+J3+L3+N3+P3</f>
@@ -1890,31 +1927,31 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -1926,31 +1963,31 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="3">
         <v>4</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S5" s="3">
         <f>H5+J5+L5+N5+P5</f>
@@ -1959,22 +1996,22 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="3">
         <v>3</v>
@@ -1986,25 +2023,25 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -2016,37 +2053,37 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" si="0"/>
@@ -2055,25 +2092,25 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3">
         <v>3</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S9" s="3">
         <f t="shared" si="0"/>
@@ -2082,19 +2119,19 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="3">
         <v>3</v>
@@ -2106,31 +2143,31 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="Q11" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="R11" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="S11" s="3">
         <f t="shared" si="0"/>
@@ -2139,40 +2176,40 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="R12" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="S12" s="3">
         <f t="shared" si="0"/>
@@ -2181,28 +2218,28 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S13" s="3">
         <f t="shared" si="0"/>
@@ -2211,25 +2248,25 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="3">
         <v>4</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="0"/>
@@ -2238,16 +2275,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S15" s="3">
         <f t="shared" si="0"/>
@@ -2256,7 +2293,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S16" s="3">
         <f t="shared" si="0"/>
@@ -2265,19 +2302,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2289,7 +2326,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S18" s="3">
         <f t="shared" si="0"/>
@@ -2298,7 +2335,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="0"/>
@@ -2307,7 +2344,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S20" s="3">
         <f t="shared" si="0"/>
@@ -2316,7 +2353,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S21" s="3">
         <f t="shared" si="0"/>
@@ -2325,7 +2362,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S22" s="3">
         <f t="shared" si="0"/>
@@ -2334,7 +2371,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S23" s="3">
         <f t="shared" si="0"/>
@@ -2343,7 +2380,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S24" s="3">
         <f t="shared" si="0"/>
@@ -2352,13 +2389,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="Q25" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S25" s="3">
         <f t="shared" si="0"/>
@@ -2430,7 +2467,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2476,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -2485,7 +2522,7 @@
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>27</v>
@@ -2499,13 +2536,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2516,13 +2553,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2533,27 +2570,27 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2588,13 +2625,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
@@ -2602,13 +2639,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
@@ -2616,13 +2653,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -2630,13 +2667,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -2644,53 +2681,53 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>76</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="3">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2724,132 +2761,132 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2877,145 +2914,145 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
         <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>61</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" t="s">
         <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
         <v>64</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3041,19 +3078,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3071,7 +3108,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3084,7 +3121,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,7 +3134,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3115,7 +3152,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jobs cards are at a stable place
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="230">
   <si>
     <t>Name</t>
   </si>
@@ -387,9 +387,6 @@
     <t>SEEN IT ALL%nDoes not panic due to Victim situations.%n %nMEDICAL TRAINING%nMay add 🔍 to any action with ➕ for 1 ⚡</t>
   </si>
   <si>
-    <t>LEADER%nEvery colleague loses 1 point of Panic at the beginning of each round when outside with the Chief%n %nINSPIRATIONAL%nMay give ⚡⚡⚡ to a colleague for a cost of ⚡⚡⚡⚡</t>
-  </si>
-  <si>
     <t>Examine%n➜👁👁🔍🔍</t>
   </si>
   <si>
@@ -709,6 +706,15 @@
   </si>
   <si>
     <t>Civilian</t>
+  </si>
+  <si>
+    <t>Inspire%n(see below)</t>
+  </si>
+  <si>
+    <t>Quick Remedy%n➜ ➕</t>
+  </si>
+  <si>
+    <t>LEADER%nColleagues lose 1 Panic when they begin a round outside with the Chief%n %nINSPIRE%nMay give ⚡⚡⚡ to a colleague.</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1081,8 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>29</v>
@@ -1199,7 +1205,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N2" s="3">
         <v>3</v>
@@ -1287,7 +1293,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -1311,16 +1317,16 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>95</v>
+        <v>228</v>
       </c>
       <c r="L4" s="3">
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>105</v>
+        <v>227</v>
       </c>
       <c r="N4" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O4" t="s">
         <v>80</v>
@@ -1335,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>120</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1346,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D5" s="3">
         <v>5</v>
@@ -1364,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>228</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1405,7 +1411,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1464,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1500,7 +1506,7 @@
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P7" s="3">
         <v>4</v>
@@ -1523,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -1559,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P8" s="3">
         <v>5</v>
@@ -1579,7 +1585,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" s="3">
         <v>8</v>
@@ -1633,7 +1639,7 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 I5:I9 Q2:Q9 M2:M9 I3 O2:O9 K2:K7 K9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 K9 Q2:Q9 M2:M9 I3 O2:O9 K2:K7 I5:I9">
       <formula1>Action</formula1>
     </dataValidation>
   </dataValidations>
@@ -1647,7 +1653,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -1673,71 +1679,71 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
         <v>185</v>
-      </c>
-      <c r="D4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
         <v>187</v>
-      </c>
-      <c r="D5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" t="s">
         <v>190</v>
-      </c>
-      <c r="B7" t="s">
-        <v>191</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" t="s">
         <v>193</v>
-      </c>
-      <c r="D8" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
@@ -1746,15 +1752,15 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" t="s">
         <v>198</v>
-      </c>
-      <c r="D11" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1773,7 +1779,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,75 +1811,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>42</v>
@@ -1882,10 +1888,10 @@
         <v>2</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S2" s="3">
         <f>H2+J2+L2+N2+P2</f>
@@ -1894,19 +1900,19 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>42</v>
@@ -1915,10 +1921,10 @@
         <v>2</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S3" s="3">
         <f t="shared" ref="S3:S25" si="0">H3+J3+L3+N3+P3</f>
@@ -1927,22 +1933,22 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>42</v>
@@ -1963,19 +1969,19 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>42</v>
@@ -1984,10 +1990,10 @@
         <v>4</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S5" s="3">
         <f>H5+J5+L5+N5+P5</f>
@@ -1996,19 +2002,19 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>44</v>
@@ -2023,22 +2029,22 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>44</v>
@@ -2053,22 +2059,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>44</v>
@@ -2083,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" si="0"/>
@@ -2092,16 +2098,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>32</v>
@@ -2110,7 +2116,7 @@
         <v>3</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S9" s="3">
         <f t="shared" si="0"/>
@@ -2119,16 +2125,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>32</v>
@@ -2143,19 +2149,19 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>59</v>
@@ -2164,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="Q11" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="R11" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="S11" s="3">
         <f t="shared" si="0"/>
@@ -2176,25 +2182,25 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H12" s="3">
         <v>3</v>
@@ -2206,10 +2212,10 @@
         <v>2</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S12" s="3">
         <f t="shared" si="0"/>
@@ -2218,19 +2224,19 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>57</v>
@@ -2239,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S13" s="3">
         <f t="shared" si="0"/>
@@ -2248,16 +2254,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>32</v>
@@ -2266,7 +2272,7 @@
         <v>4</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="0"/>
@@ -2275,16 +2281,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="S15" s="3">
         <f t="shared" si="0"/>
@@ -2293,7 +2299,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S16" s="3">
         <f t="shared" si="0"/>
@@ -2302,16 +2308,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>44</v>
@@ -2326,7 +2332,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S18" s="3">
         <f t="shared" si="0"/>
@@ -2335,7 +2341,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="0"/>
@@ -2344,7 +2350,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S20" s="3">
         <f t="shared" si="0"/>
@@ -2353,7 +2359,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S21" s="3">
         <f t="shared" si="0"/>
@@ -2362,7 +2368,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S22" s="3">
         <f t="shared" si="0"/>
@@ -2371,7 +2377,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S23" s="3">
         <f t="shared" si="0"/>
@@ -2380,7 +2386,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S24" s="3">
         <f t="shared" si="0"/>
@@ -2389,13 +2395,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="Q25" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S25" s="3">
         <f t="shared" si="0"/>
@@ -2467,7 +2473,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2576,7 +2582,7 @@
         <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2590,7 +2596,7 @@
         <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2625,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
@@ -2659,7 +2665,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -2704,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2715,7 +2721,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -3078,19 +3084,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3108,7 +3114,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3121,7 +3127,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3134,7 +3140,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3152,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting work on situations
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jobs" sheetId="1" r:id="rId1"/>
@@ -657,9 +657,6 @@
     <t>URGENT: Unless handled, add Extinguish each round. EMERGENCY: Unless handled, add 2 Extinguish and 1 Panic to each responder on card.</t>
   </si>
   <si>
-    <t>URGENT: Unless Handled, add 1 Treat each Round. Max 5 Treat actions.</t>
-  </si>
-  <si>
     <t>Cannot treat the victim until they are cleared. URGENT: Unless Handled, add 1 Treat each round</t>
   </si>
   <si>
@@ -675,9 +672,6 @@
     <t>Final Round</t>
   </si>
   <si>
-    <t>Reveal all cards when this is revealed. Must Extinguish all flames by end of Final Round</t>
-  </si>
-  <si>
     <t>Unless handled, add 1 Extinguish every round</t>
   </si>
   <si>
@@ -715,6 +709,12 @@
   </si>
   <si>
     <t>LEADER%nColleagues lose 1 Panic when they begin a round outside with the Chief%n %nINSPIRE%nMay give ⚡⚡⚡ to a colleague.</t>
+  </si>
+  <si>
+    <t>URGENT: Unless Handled, add 1 Treat each Round</t>
+  </si>
+  <si>
+    <t>Reveal all cards when this is revealed. Must Extinguish all flames by end of Final Round, otherwise lose scenario</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="S4" sqref="S4"/>
     </sheetView>
@@ -1293,7 +1293,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -1317,13 +1317,13 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L4" s="3">
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N4" s="3">
         <v>4</v>
@@ -1341,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" s="3">
         <v>5</v>
@@ -1370,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -1411,7 +1411,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1470,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1529,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -1585,7 +1585,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D9" s="3">
         <v>8</v>
@@ -1711,7 +1711,7 @@
         <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>147</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -2089,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" si="0"/>
@@ -2149,13 +2149,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>138</v>
@@ -2212,7 +2212,7 @@
         <v>2</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R12" s="5" t="s">
         <v>145</v>
@@ -2245,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S13" s="3">
         <f t="shared" si="0"/>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -2272,7 +2272,7 @@
         <v>4</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="0"/>
@@ -2290,7 +2290,7 @@
         <v>172</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S15" s="3">
         <f t="shared" si="0"/>
@@ -2401,7 +2401,7 @@
         <v>176</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="S25" s="3">
         <f t="shared" si="0"/>
@@ -3158,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>